<commit_message>
Dados processados, MER e relacional atualizados
</commit_message>
<xml_diff>
--- a/Dados_processados_sample.xlsx
+++ b/Dados_processados_sample.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PCMonstro\Desktop\Sistema-de-analise-de-dados-abertos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E36373FC-0B42-4863-808C-D9F57894ACE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBC9B11A-0950-488E-AD51-4D81E979C2E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11760" xr2:uid="{72A0A92A-7D5D-46D5-A79A-A794DD2E7976}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="155">
   <si>
     <t>Despesas</t>
   </si>
@@ -365,9 +365,6 @@
     <t>16.519.676/0001-26</t>
   </si>
   <si>
-    <t xml:space="preserve">015.542.835/74  -  </t>
-  </si>
-  <si>
     <t>Leur</t>
   </si>
   <si>
@@ -456,16 +453,65 @@
   </si>
   <si>
     <t>atividade</t>
+  </si>
+  <si>
+    <t>CONDE &amp; DELL ARINGA - DES DE SOFTWARES</t>
+  </si>
+  <si>
+    <t>MASTER TOWER</t>
+  </si>
+  <si>
+    <t>AUTO POSTO ROMAFS LT</t>
+  </si>
+  <si>
+    <t>FRANCISCO RESTAURANTE LTDA EPP</t>
+  </si>
+  <si>
+    <t>3L COMERCIO DE COMBUSTIVEIS E LUBRIFICANTES LTDA</t>
+  </si>
+  <si>
+    <t>PAROLE COMUNICALÇAO E SERVIÇOS</t>
+  </si>
+  <si>
+    <t>DIVULGAÇÃO DA ATIVIDADE PARLAMENTAR.</t>
+  </si>
+  <si>
+    <t>GOL LINHAS AÉREAS INTELIGENTES</t>
+  </si>
+  <si>
+    <t>015.542.835/0074-0</t>
+  </si>
+  <si>
+    <t>LUCAS GEDEON SAMPAIO</t>
+  </si>
+  <si>
+    <t>IRACEMA LOURENÇO SANTOS RODRIGUES - ME</t>
+  </si>
+  <si>
+    <t>VIA BAHIA</t>
+  </si>
+  <si>
+    <t>Legislatura</t>
+  </si>
+  <si>
+    <t>ano</t>
+  </si>
+  <si>
+    <t>dt_ini</t>
+  </si>
+  <si>
+    <t>dt_fim</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="###0.00"/>
     <numFmt numFmtId="165" formatCode="00000000000"/>
-    <numFmt numFmtId="170" formatCode="0000000"/>
+    <numFmt numFmtId="166" formatCode="0000000"/>
+    <numFmt numFmtId="167" formatCode="000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -520,7 +566,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -533,8 +579,10 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -850,16 +898,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34C86A1C-937C-4B5C-AA9A-002F63729E20}">
-  <dimension ref="A1:R113"/>
+  <dimension ref="A1:R143"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F149" sqref="F149"/>
+    <sheetView tabSelected="1" topLeftCell="A123" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D134" sqref="A129:D134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
@@ -1098,7 +1146,7 @@
         <v>7068069</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>109</v>
+        <v>147</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>76</v>
@@ -1121,7 +1169,7 @@
         <v>7030654</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>12</v>
@@ -1133,7 +1181,7 @@
         <v>43862</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G12" s="8">
         <v>188</v>
@@ -1144,7 +1192,7 @@
         <v>7138203</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>16</v>
@@ -2043,10 +2091,10 @@
         <v>87594749120</v>
       </c>
       <c r="C65" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D65" t="s">
         <v>110</v>
-      </c>
-      <c r="D65" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -2057,10 +2105,10 @@
         <v>83146270463</v>
       </c>
       <c r="C66" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="D66" t="s">
         <v>114</v>
-      </c>
-      <c r="D66" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -2071,7 +2119,7 @@
         <v>19530773587</v>
       </c>
       <c r="C67" s="8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D67" t="s">
         <v>66</v>
@@ -2079,18 +2127,18 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B70" t="s">
         <v>61</v>
       </c>
       <c r="C70" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -2098,10 +2146,10 @@
         <v>5573</v>
       </c>
       <c r="B71" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C71">
-        <v>492</v>
+        <v>55</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -2109,10 +2157,10 @@
         <v>5154</v>
       </c>
       <c r="B72" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C72">
-        <v>487</v>
+        <v>54</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -2120,10 +2168,10 @@
         <v>4981</v>
       </c>
       <c r="B73" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C73">
-        <v>515</v>
+        <v>55</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -2131,10 +2179,10 @@
         <v>5918</v>
       </c>
       <c r="B74" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C74">
-        <v>526</v>
+        <v>56</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -2142,10 +2190,10 @@
         <v>5625</v>
       </c>
       <c r="B75" s="13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C75">
-        <v>497</v>
+        <v>55</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -2153,10 +2201,10 @@
         <v>6026</v>
       </c>
       <c r="B76" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C76">
-        <v>578</v>
+        <v>56</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -2164,10 +2212,10 @@
         <v>5170</v>
       </c>
       <c r="B77" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C77">
-        <v>451</v>
+        <v>54</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
@@ -2175,10 +2223,10 @@
         <v>5140</v>
       </c>
       <c r="B78" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C78">
-        <v>485</v>
+        <v>54</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
@@ -2186,10 +2234,10 @@
         <v>5923</v>
       </c>
       <c r="B79" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C79">
-        <v>522</v>
+        <v>56</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
@@ -2197,44 +2245,44 @@
         <v>5982</v>
       </c>
       <c r="B80" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C80">
-        <v>559</v>
+        <v>56</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B83" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84">
-        <v>492</v>
+        <v>578</v>
       </c>
       <c r="B84">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85">
-        <v>487</v>
+        <v>559</v>
       </c>
       <c r="B85">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86">
-        <v>515</v>
+        <v>526</v>
       </c>
       <c r="B86">
         <v>55</v>
@@ -2242,159 +2290,484 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87">
-        <v>526</v>
+        <v>515</v>
       </c>
       <c r="B87">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88">
-        <v>497</v>
+        <v>502</v>
       </c>
       <c r="B88">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89">
-        <v>578</v>
-      </c>
-      <c r="B89">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90">
-        <v>451</v>
-      </c>
-      <c r="B90">
-        <v>54</v>
+      <c r="A90" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91">
-        <v>485</v>
-      </c>
-      <c r="B91">
-        <v>54</v>
+      <c r="A91" t="s">
+        <v>118</v>
+      </c>
+      <c r="B91" t="s">
+        <v>61</v>
+      </c>
+      <c r="C91" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92">
-        <v>522</v>
+        <v>2227</v>
       </c>
       <c r="B92">
+        <v>12133728368</v>
+      </c>
+      <c r="C92">
         <v>56</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93">
-        <v>559</v>
+        <v>3163</v>
       </c>
       <c r="B93">
+        <v>28008901187</v>
+      </c>
+      <c r="C93">
         <v>56</v>
       </c>
     </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>2917</v>
+      </c>
+      <c r="B94" s="9">
+        <v>28022995819</v>
+      </c>
+      <c r="C94">
+        <v>56</v>
+      </c>
+    </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
-        <v>131</v>
+      <c r="A95">
+        <v>995</v>
+      </c>
+      <c r="B95" s="9">
+        <v>29474485534</v>
+      </c>
+      <c r="C95">
+        <v>56</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
-        <v>119</v>
-      </c>
-      <c r="B96" t="s">
-        <v>61</v>
-      </c>
-      <c r="C96" t="s">
-        <v>132</v>
+      <c r="A96">
+        <v>1071</v>
+      </c>
+      <c r="B96" s="9">
+        <v>4789113515</v>
+      </c>
+      <c r="C96">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>233</v>
+      </c>
+      <c r="B97" s="9">
+        <v>66728983791</v>
+      </c>
+      <c r="C97">
+        <v>56</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
+      <c r="A98">
+        <v>1422</v>
+      </c>
+      <c r="B98" s="9">
+        <v>4251091191</v>
+      </c>
+      <c r="C98">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>733</v>
+      </c>
+      <c r="B99" s="9">
+        <v>43428169700</v>
+      </c>
+      <c r="C99">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>3345</v>
+      </c>
+      <c r="B100" s="9">
+        <v>87594749120</v>
+      </c>
+      <c r="C100">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>3090</v>
+      </c>
+      <c r="B101" s="9">
+        <v>83146270463</v>
+      </c>
+      <c r="C101">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>2938</v>
+      </c>
+      <c r="B102" s="8">
+        <v>19530773587</v>
+      </c>
+      <c r="C102">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>1822</v>
+      </c>
+      <c r="B103">
+        <v>53467108415</v>
+      </c>
+      <c r="C103">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>3072</v>
+      </c>
+      <c r="B104" s="6">
+        <v>3380916889</v>
+      </c>
+      <c r="C104">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>133</v>
+      </c>
+      <c r="B107" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <v>115</v>
+      </c>
+      <c r="B108">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109">
+        <v>112</v>
+      </c>
+      <c r="B109">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110">
+        <v>100</v>
+      </c>
+      <c r="B110">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" s="14">
+        <v>96</v>
+      </c>
+      <c r="B111">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112" s="14">
+        <v>94</v>
+      </c>
+      <c r="B112">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
-        <v>134</v>
-      </c>
-      <c r="B99" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
+      <c r="B115" t="s">
         <v>137</v>
       </c>
-      <c r="B102" t="s">
+      <c r="C115" t="s">
         <v>138</v>
       </c>
-      <c r="C102" t="s">
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B116" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A103" s="8" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A104" s="8" t="s">
+      <c r="C116" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117" s="8" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A105" s="8" t="s">
+      <c r="B117" t="s">
+        <v>140</v>
+      </c>
+      <c r="C117" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118" s="8" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A106" s="8" t="s">
+      <c r="B118" t="s">
+        <v>141</v>
+      </c>
+      <c r="C118" s="8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" s="8" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A107" s="8" t="s">
+      <c r="B119" t="s">
+        <v>142</v>
+      </c>
+      <c r="C119" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120" s="8" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A108" s="8" t="s">
+      <c r="B120" t="s">
+        <v>143</v>
+      </c>
+      <c r="C120" s="8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121" s="8" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A109" s="8" t="s">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122" s="8" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A110" s="8" t="s">
+      <c r="B122" t="s">
+        <v>144</v>
+      </c>
+      <c r="C122" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A123" s="8" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A111" s="8" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A112" s="8" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A113" s="8" t="s">
-        <v>116</v>
-      </c>
+      <c r="B123" t="s">
+        <v>146</v>
+      </c>
+      <c r="C123" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A124" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="B124" t="s">
+        <v>148</v>
+      </c>
+      <c r="C124" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A125" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="B125" t="s">
+        <v>149</v>
+      </c>
+      <c r="C125" s="8" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A126" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="B126" t="s">
+        <v>150</v>
+      </c>
+      <c r="C126" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>152</v>
+      </c>
+      <c r="B129" t="s">
+        <v>118</v>
+      </c>
+      <c r="C129" t="s">
+        <v>153</v>
+      </c>
+      <c r="D129" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A130">
+        <v>2022</v>
+      </c>
+      <c r="B130">
+        <v>57</v>
+      </c>
+      <c r="C130" s="15">
+        <v>44958</v>
+      </c>
+      <c r="D130" s="15">
+        <v>46418</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A131">
+        <v>2018</v>
+      </c>
+      <c r="B131">
+        <v>56</v>
+      </c>
+      <c r="C131" s="15">
+        <v>43497</v>
+      </c>
+      <c r="D131" s="15">
+        <v>44957</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A132">
+        <v>2014</v>
+      </c>
+      <c r="B132">
+        <v>55</v>
+      </c>
+      <c r="C132" s="15">
+        <v>42036</v>
+      </c>
+      <c r="D132" s="15">
+        <v>43496</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A133">
+        <v>2010</v>
+      </c>
+      <c r="B133">
+        <v>54</v>
+      </c>
+      <c r="C133" s="15">
+        <v>40575</v>
+      </c>
+      <c r="D133" s="15">
+        <v>42035</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A134">
+        <v>2006</v>
+      </c>
+      <c r="B134">
+        <v>53</v>
+      </c>
+      <c r="C134" s="15">
+        <v>39114</v>
+      </c>
+      <c r="D134" s="15">
+        <v>40574</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A135" s="8"/>
+      <c r="C135" s="8"/>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A136" s="8"/>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A137" s="8"/>
+      <c r="C137" s="8"/>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A138" s="8"/>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A139" s="8"/>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A140" s="8"/>
+      <c r="C140" s="8"/>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A141" s="8"/>
+      <c r="C141" s="8"/>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A142" s="8"/>
+      <c r="C142" s="8"/>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A143" s="8"/>
+      <c r="C143" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>